<commit_message>
Update sample_data.xlsx and add sample_data_full.sql
</commit_message>
<xml_diff>
--- a/data/sample_data.xlsx
+++ b/data/sample_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\CITS5206 Capstone Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39CB5DC-E6CC-4C70-AF23-D963BD8BE51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DD6B29-F04C-4839-92C8-56EC056A0A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTPScholarships" sheetId="16" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="143">
   <si>
     <t>E330_AttendanceTypeCode</t>
   </si>
@@ -131,18 +131,6 @@
     <t>E310_CourseOfStudyType</t>
   </si>
   <si>
-    <t>7d7f274c624b1e9d451b4e33ea6077b72df610749e544f03031dea27af2ca978</t>
-  </si>
-  <si>
-    <t>46f6e455781db7b75661689f3f13d4cf275dc45dca274f835c2da0f93c84c768</t>
-  </si>
-  <si>
-    <t>81409a9914e1c8b8661a2125f12f1e5cd1c7b5580379fc9f0f3aac7c2896d907</t>
-  </si>
-  <si>
-    <t>0451da5f7c51e403d6d52d75350eaf6adda1c11807fad8bbe009a6b7113857ee</t>
-  </si>
-  <si>
     <t>E463_SpecialisationCode</t>
   </si>
   <si>
@@ -158,54 +146,12 @@
     <t>UID46_EarlyExitAwardsResKey</t>
   </si>
   <si>
-    <t>a10c042ad5eb7da7fd6326a2f32e897d9358de42f8b21f853999a690b914533f</t>
-  </si>
-  <si>
-    <t>5c86a1d5895879805218301170d71872897592999d81b894ef79327b5b7170e1</t>
-  </si>
-  <si>
-    <t>b20e18623cc1e401ab90922f5dd101cabbf89976062f438e6af5ec5b6a2f8b41</t>
-  </si>
-  <si>
-    <t>a236dc5baa1c9ef75d0a640d96963ee11bbf1ee0a22444dd326f9744d30ea788</t>
-  </si>
-  <si>
-    <t>c6a33a78afb3c4c6d1c7995e30ee32fc1a41eb7223c7876576c1464dff5d3bc0</t>
-  </si>
-  <si>
-    <t>b1f575332da47cb6061fc0cb997da217dc1b79347aaabea6976c79d35cdc1e4d</t>
-  </si>
-  <si>
-    <t>fbe1885ce76930adbe74f61f9e05925cc3b4d687113bd7e00cb68db3c7da6e4e</t>
-  </si>
-  <si>
-    <t>9d98125deaf9879483495282db6fb1c13511d307137559e0858a99f78b124d84</t>
-  </si>
-  <si>
-    <t>e9e34cf9e6be04b58eb9c48e83cfc79b5153831f709b123fe08db3c361f15847</t>
-  </si>
-  <si>
     <t>E327_BasisForAdmissionCode</t>
   </si>
   <si>
     <t>UID17_BasisForAdmissionResKey</t>
   </si>
   <si>
-    <t>4bdd6657e8a65a5526b1cae8b334470859ce9982cbddb3b86f69bae10c0797f9</t>
-  </si>
-  <si>
-    <t>63c6bdb49d8a7e91e2d02db148b9ea4c80492d49930a6eda4bdd3ca70944b4cf</t>
-  </si>
-  <si>
-    <t>d76a8e187e39247bbbd72b891ccac0ab6dd99b73c8646ea3d9cb3a3837dfcef0</t>
-  </si>
-  <si>
-    <t>de18642ab7b58283158c7fde12d0c9f33ed6cff49c61a2c6c2bcef38f6418f79</t>
-  </si>
-  <si>
-    <t>1352130a9bf0fc648ea4d52b769db6e5d9a5ac51c39e8a35881feab327903e9e</t>
-  </si>
-  <si>
     <t>E595_HDRSecondaryFieldOfResearchCode</t>
   </si>
   <si>
@@ -296,18 +242,6 @@
     <t>COMMITTED</t>
   </si>
   <si>
-    <t>75e0280303f9379a28139ac0d34b027ffe17d959441186c4014fd1e0d10caf8e</t>
-  </si>
-  <si>
-    <t>63d839cca661b050944a3bf8c957a4d2d01dc056474a84d05cd7bce9091bf872</t>
-  </si>
-  <si>
-    <t>abcad50b662dde3421586acbec650638f9d37fd320c741f9ef966deffab88cbd</t>
-  </si>
-  <si>
-    <t>410e500e563ca4909deb547b1e582589bbb4002e37a942f52a95ad009012f82b</t>
-  </si>
-  <si>
     <t>E558_HELPLoanAmount</t>
   </si>
   <si>
@@ -383,9 +317,6 @@
     <t>ACTIVE</t>
   </si>
   <si>
-    <t>c6a33a78af…ff5d3bc0</t>
-  </si>
-  <si>
     <t>CA</t>
   </si>
   <si>
@@ -399,16 +330,160 @@
   </si>
   <si>
     <t>STIP001</t>
+  </si>
+  <si>
+    <t>STU100003</t>
+  </si>
+  <si>
+    <t>STU100001</t>
+  </si>
+  <si>
+    <t>STU100002</t>
+  </si>
+  <si>
+    <t>STU100004</t>
+  </si>
+  <si>
+    <t>CA001</t>
+  </si>
+  <si>
+    <t>SL001</t>
+  </si>
+  <si>
+    <t>SL002</t>
+  </si>
+  <si>
+    <t>SL003</t>
+  </si>
+  <si>
+    <t>SL004</t>
+  </si>
+  <si>
+    <t>ADM001</t>
+  </si>
+  <si>
+    <t>ADM002</t>
+  </si>
+  <si>
+    <t>ADM003</t>
+  </si>
+  <si>
+    <t>ADM004</t>
+  </si>
+  <si>
+    <t>CRS001</t>
+  </si>
+  <si>
+    <t>CRS002</t>
+  </si>
+  <si>
+    <t>CRS003</t>
+  </si>
+  <si>
+    <t>CRS004</t>
+  </si>
+  <si>
+    <t>EXIT001</t>
+  </si>
+  <si>
+    <t>EXIT002</t>
+  </si>
+  <si>
+    <t>EXIT003</t>
+  </si>
+  <si>
+    <t>EXIT004</t>
+  </si>
+  <si>
+    <t>CSR001</t>
+  </si>
+  <si>
+    <t>CSR002</t>
+  </si>
+  <si>
+    <t>CSR003</t>
+  </si>
+  <si>
+    <t>CSR004</t>
+  </si>
+  <si>
+    <t>CRD001</t>
+  </si>
+  <si>
+    <t>CRD002</t>
+  </si>
+  <si>
+    <t>CRD003</t>
+  </si>
+  <si>
+    <t>CRD004</t>
+  </si>
+  <si>
+    <t>SPC001</t>
+  </si>
+  <si>
+    <t>SPC002</t>
+  </si>
+  <si>
+    <t>SPC003</t>
+  </si>
+  <si>
+    <t>SPC004</t>
+  </si>
+  <si>
+    <t>RTP001</t>
+  </si>
+  <si>
+    <t>CSP001</t>
+  </si>
+  <si>
+    <t>CSP002</t>
+  </si>
+  <si>
+    <t>CSP003</t>
+  </si>
+  <si>
+    <t>CSP004</t>
+  </si>
+  <si>
+    <t>BAS001</t>
+  </si>
+  <si>
+    <t>BAS002</t>
+  </si>
+  <si>
+    <t>BAS003</t>
+  </si>
+  <si>
+    <t>BAS004</t>
+  </si>
+  <si>
+    <t>FOE001</t>
+  </si>
+  <si>
+    <t>FOE002</t>
+  </si>
+  <si>
+    <t>FOE003</t>
+  </si>
+  <si>
+    <t>FOE004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -448,7 +523,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -729,38 +804,41 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>107</v>
       </c>
-      <c r="E1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
+      <c r="B2" t="s">
+        <v>130</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -782,97 +860,98 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="1" max="2" width="31.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
       <c r="C1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2">
-        <v>238225</v>
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
       </c>
       <c r="C2">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3">
-        <v>8081801</v>
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
       </c>
       <c r="C3">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4">
-        <v>7532867</v>
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
       </c>
       <c r="C4">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>7546262</v>
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
       </c>
       <c r="C5">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B87A80-9EA1-4F94-8A68-D1B902C13A43}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -881,12 +960,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5780</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -895,7 +974,50 @@
         <v>44602</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45092</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45741</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45626</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -905,72 +1027,73 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2">
-        <v>1076927</v>
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
       </c>
       <c r="C2">
         <v>90900</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3">
-        <v>3458114</v>
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
       </c>
       <c r="C3">
         <v>90701</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>3458115</v>
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
       </c>
       <c r="C4">
         <v>91500</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>1080279</v>
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
       </c>
       <c r="C5">
         <v>90900</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -980,20 +1103,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1013,9 +1136,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1462</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -1033,9 +1156,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1463</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>119</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -1053,9 +1176,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1464</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>120</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -1073,9 +1196,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1465</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>121</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -1103,27 +1226,27 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" customWidth="1"/>
-    <col min="11" max="11" width="40.28515625" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.5546875" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" customWidth="1"/>
+    <col min="11" max="11" width="40.33203125" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1143,12 +1266,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>8710</v>
-      </c>
-      <c r="B2">
-        <v>200916</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
       </c>
       <c r="C2">
         <v>91901</v>
@@ -1163,12 +1286,12 @@
         <v>39082</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>8710</v>
-      </c>
-      <c r="B3">
-        <v>200917</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
       </c>
       <c r="C3">
         <v>91901</v>
@@ -1183,12 +1306,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8735</v>
-      </c>
-      <c r="B4">
-        <v>200926</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
       </c>
       <c r="C4">
         <v>61799</v>
@@ -1203,12 +1326,12 @@
         <v>39082</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8735</v>
-      </c>
-      <c r="B5">
-        <v>200927</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
       </c>
       <c r="C5">
         <v>61799</v>
@@ -1224,6 +1347,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1233,33 +1357,33 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" customWidth="1"/>
-    <col min="14" max="14" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" customWidth="1"/>
+    <col min="12" max="12" width="24.44140625" customWidth="1"/>
+    <col min="13" max="13" width="27.88671875" customWidth="1"/>
+    <col min="14" max="14" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -1277,15 +1401,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1">
         <v>45597</v>
@@ -1294,21 +1418,21 @@
         <v>45626</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1002</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1">
         <v>45597</v>
@@ -1317,10 +1441,10 @@
         <v>45488</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1333,37 +1457,37 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="C2">
         <v>28000</v>
@@ -1382,27 +1506,27 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
@@ -1411,12 +1535,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10070</v>
-      </c>
-      <c r="B2">
-        <v>7841</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
       </c>
       <c r="C2">
         <v>22</v>
@@ -1428,12 +1552,12 @@
         <v>39447</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10070</v>
-      </c>
-      <c r="B3">
-        <v>7835</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
       </c>
       <c r="C3">
         <v>22</v>
@@ -1445,12 +1569,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10267</v>
-      </c>
-      <c r="B4">
-        <v>3831</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
       </c>
       <c r="C4">
         <v>22</v>
@@ -1462,12 +1586,12 @@
         <v>39082</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10267</v>
-      </c>
-      <c r="B5">
-        <v>954</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
       </c>
       <c r="C5">
         <v>22</v>
@@ -1480,6 +1604,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1489,57 +1614,57 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1">
         <v>43617</v>
@@ -1557,18 +1682,18 @@
         <v>151.5</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1">
         <v>43405</v>
@@ -1586,18 +1711,18 @@
         <v>149</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>86</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1">
         <v>43617</v>
@@ -1615,18 +1740,18 @@
         <v>151.5</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>85</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1">
         <v>43252</v>
@@ -1644,13 +1769,14 @@
         <v>149</v>
       </c>
       <c r="H5" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1660,94 +1786,94 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1"/>
-    <col min="8" max="8" width="47.5703125" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.44140625" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="8" max="8" width="47.5546875" customWidth="1"/>
+    <col min="9" max="9" width="27.5546875" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="J1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="K1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="M1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1">
         <v>45337</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1">
         <v>45352</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="H2" s="1">
         <v>45356</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="J2">
         <v>4000</v>
@@ -1756,10 +1882,10 @@
         <v>120</v>
       </c>
       <c r="L2" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="M2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1771,49 +1897,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA884D7-638B-4AF2-8180-9F36274BF0D4}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="D2" s="5">
         <v>45352</v>
@@ -1825,7 +1951,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="4"/>
@@ -1840,21 +1966,21 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="34.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1865,10 +1991,10 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
@@ -1877,12 +2003,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1462</v>
-      </c>
-      <c r="B2">
-        <v>8849</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
       </c>
       <c r="C2">
         <v>201</v>
@@ -1900,12 +2026,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1463</v>
-      </c>
-      <c r="B3">
-        <v>8949</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
       </c>
       <c r="C3">
         <v>302</v>
@@ -1923,12 +2049,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1463</v>
-      </c>
-      <c r="B4">
-        <v>8973</v>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
       <c r="C4">
         <v>301</v>
@@ -1946,12 +2072,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1464</v>
-      </c>
-      <c r="B5">
-        <v>8923</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
       </c>
       <c r="C5">
         <v>401</v>
@@ -1970,6 +2096,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1978,59 +2105,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB82313-DE9E-4BFD-A697-48AD02FC9558}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2">
-        <v>2839074</v>
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
       </c>
       <c r="C2">
         <v>0.25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>3001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>951277</v>
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -2042,12 +2169,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4">
-        <v>1834951</v>
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
       </c>
       <c r="C4">
         <v>2.4990000000000001</v>
@@ -2059,12 +2186,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5">
-        <v>1845360</v>
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2077,6 +2204,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2086,28 +2214,28 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" customWidth="1"/>
-    <col min="10" max="10" width="35.7109375" customWidth="1"/>
-    <col min="11" max="11" width="37.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="11" max="11" width="37.88671875" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" customWidth="1"/>
+    <col min="13" max="13" width="26.44140625" customWidth="1"/>
     <col min="14" max="14" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2115,7 +2243,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -2127,48 +2255,48 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="L1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="M1" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="N1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2">
-        <v>8725</v>
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="D2" s="1">
-        <v>40575</v>
+        <v>43525</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
+      <c r="F2" s="1">
+        <v>45245</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -2179,8 +2307,8 @@
       <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
-        <v>10</v>
+      <c r="J2">
+        <v>1001</v>
       </c>
       <c r="K2" t="s">
         <v>10</v>
@@ -2195,15 +2323,15 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3">
-        <v>8725</v>
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1">
         <v>40602</v>
@@ -2226,8 +2354,8 @@
       <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
-        <v>10</v>
+      <c r="K3">
+        <v>1100</v>
       </c>
       <c r="L3">
         <v>202409</v>
@@ -2239,15 +2367,15 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4">
-        <v>8725</v>
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="D4" s="1">
         <v>39845</v>
@@ -2267,8 +2395,8 @@
       <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
-        <v>10</v>
+      <c r="J4">
+        <v>1002</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
@@ -2283,15 +2411,15 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>8725</v>
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="D5" s="1">
         <v>39867</v>
@@ -2314,8 +2442,8 @@
       <c r="J5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
-        <v>10</v>
+      <c r="K5">
+        <v>1200</v>
       </c>
       <c r="L5">
         <v>202412</v>
@@ -2328,6 +2456,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>